<commit_message>
Clean up and annotate
</commit_message>
<xml_diff>
--- a/data_used/TAN1810_14C-Pico_25052020_QA_1.2.xlsx
+++ b/data_used/TAN1810_14C-Pico_25052020_QA_1.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deniseong/Documents/GitHub/TAN1810_C14/data_used/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85521C2C-8926-3F4C-BD65-D8F2C7AF965A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9EACC6-5DE2-4A47-8E64-D008BD922938}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" xr2:uid="{EA8D94A5-2552-437F-8CAB-49D88ECDE175}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="28820" windowHeight="16500" xr2:uid="{EA8D94A5-2552-437F-8CAB-49D88ECDE175}"/>
   </bookViews>
   <sheets>
     <sheet name="Complete data TAN1810" sheetId="3" r:id="rId1"/>
@@ -4006,10 +4006,10 @@
   <dimension ref="A1:AQ473"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="21" ySplit="12" topLeftCell="V285" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="21" ySplit="12" topLeftCell="V215" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="V1" sqref="V1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="E221" sqref="E221:E260"/>
+      <selection pane="bottomRight" activeCell="B224" sqref="B224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -75601,6 +75601,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005FE645E44DF4C347A076E5154A1E1A44" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03df5676f90d9b0b6eb46609cac18980">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="0e9b77c3-686e-41f8-8658-848585ae3dd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d51d7fb008a5325d8f5cab9a04c401e" ns1:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -75801,25 +75819,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAF4D0A-F01C-47D7-A5F8-17D94C30F09E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="0e9b77c3-686e-41f8-8658-848585ae3dd1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22E65951-09EC-4243-AB0C-AEAF1ED5779C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01A91921-7D0F-4824-A102-EFA4E0D9B2BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -75836,29 +75861,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22E65951-09EC-4243-AB0C-AEAF1ED5779C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAF4D0A-F01C-47D7-A5F8-17D94C30F09E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="0e9b77c3-686e-41f8-8658-848585ae3dd1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>